<commit_message>
Joker 구입후 JokerSlotView에 넣기
</commit_message>
<xml_diff>
--- a/GameData/JokerInfo.xlsx
+++ b/GameData/JokerInfo.xlsx
@@ -428,7 +428,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -484,7 +484,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>0</v>

</xml_diff>